<commit_message>
diageous - on premise and changes
</commit_message>
<xml_diff>
--- a/Projects/DIAGEOUS_SAND/Data/on_premise Template.xlsx
+++ b/Projects/DIAGEOUS_SAND/Data/on_premise Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>KPI Name</t>
   </si>
@@ -52,7 +52,13 @@
     <t>Back Bar</t>
   </si>
   <si>
+    <t>1. Back Bar</t>
+  </si>
+  <si>
     <t>Menu</t>
+  </si>
+  <si>
+    <t>1. Main Menu, Menu – Features, 3. Spirits List Menu, 4. Bottle List Menu, 5. After Dinner / Dessert Menu</t>
   </si>
 </sst>
 </file>
@@ -273,15 +279,15 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1012145748988"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="116.761133603239"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="117.82995951417"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
@@ -351,7 +357,9 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -359,11 +367,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>

</xml_diff>